<commit_message>
New Suggessions by Citrol
</commit_message>
<xml_diff>
--- a/Client-Requirements/CitrolLubricants.xlsx
+++ b/Client-Requirements/CitrolLubricants.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bug" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Production rate differs from stock ledger and stock report</t>
   </si>
@@ -35,9 +35,6 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t xml:space="preserve">Carton code should be added in local and import order </t>
-  </si>
-  <si>
     <t>Closing stock amount differs in P&amp;L A/C and Stock report</t>
   </si>
   <si>
@@ -86,12 +83,6 @@
     <t>19/9/2018</t>
   </si>
   <si>
-    <t xml:space="preserve">Need to show only Code instead of Cartoncode in Local purchase order print </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/9/2018 </t>
-  </si>
-  <si>
     <t>14/9/2018</t>
   </si>
   <si>
@@ -107,7 +98,31 @@
     <t>Difficult to see entire name of an item from the gridview which opens when pressing ctrl+L(DeliveryNote,Local and Import MRNs)</t>
   </si>
   <si>
-    <t>Tax rule issue Sales invoice</t>
+    <t>Tax rule issue in Sales invoice</t>
+  </si>
+  <si>
+    <t>17/10/2018</t>
+  </si>
+  <si>
+    <t>Import bill amount  is different form the amount in account tab</t>
+  </si>
+  <si>
+    <t>Cannot see the full name of items dispay in production and bom item's field</t>
+  </si>
+  <si>
+    <t>Want to see supplier's invoice number in purchase report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be notified when cost recalculation wizard finishes </t>
+  </si>
+  <si>
+    <t>25/11/2018</t>
+  </si>
+  <si>
+    <t>Item name instead of Itemcode in Cost recalculation wizard</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -157,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,7 +184,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,10 +509,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
@@ -503,15 +523,15 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,20 +539,31 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>25</v>
+      </c>
+      <c r="B7" s="5">
+        <v>43110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5">
         <v>43110</v>
@@ -540,10 +571,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="5">
-        <v>43111</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -554,10 +588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C18"/>
+  <dimension ref="A2:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +606,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -583,123 +617,133 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43110</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="5">
-        <v>43110</v>
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>